<commit_message>
Updated App component styles
</commit_message>
<xml_diff>
--- a/public/MADISON-BETTERLIFE-SME-RATE-CARD.xlsx
+++ b/public/MADISON-BETTERLIFE-SME-RATE-CARD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paul.kamau\Desktop\Madison BetterLife\my-app\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paul.kamau\Desktop\vite-app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39B8E21-0D56-4A9D-8589-452E9A899554}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BB3FD3-0C59-4EFB-886F-EDA6BE1315B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9525" windowHeight="7890" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9525" windowHeight="7890" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InpatientAbove18" sheetId="3" r:id="rId1"/>
@@ -3586,7 +3586,7 @@
   </sheetPr>
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -4196,7 +4196,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4258,10 +4258,9 @@
       <c r="G2" s="22">
         <v>6750</v>
       </c>
-      <c r="H2" s="24">
-        <v>1012.5</v>
-      </c>
-      <c r="I2" s="12"/>
+      <c r="H2" s="32">
+        <v>7762.5</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="19">
@@ -4285,10 +4284,9 @@
       <c r="G3" s="22">
         <v>13500</v>
       </c>
-      <c r="H3" s="24">
-        <v>2025</v>
-      </c>
-      <c r="I3" s="12"/>
+      <c r="H3" s="32">
+        <v>15525</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
@@ -4312,11 +4310,10 @@
       <c r="G4" s="22">
         <v>16875</v>
       </c>
-      <c r="H4" s="24">
-        <v>2531.25</v>
-      </c>
-      <c r="I4" s="12"/>
-      <c r="L4" s="32"/>
+      <c r="H4" s="32">
+        <v>19406.25</v>
+      </c>
+      <c r="K4" s="32"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
@@ -4340,11 +4337,10 @@
       <c r="G5" s="22">
         <v>20250</v>
       </c>
-      <c r="H5" s="24">
-        <v>3037.5</v>
-      </c>
-      <c r="I5" s="12"/>
-      <c r="L5" s="32"/>
+      <c r="H5" s="32">
+        <v>23287.5</v>
+      </c>
+      <c r="K5" s="32"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
@@ -4368,11 +4364,10 @@
       <c r="G6" s="22">
         <v>23625</v>
       </c>
-      <c r="H6" s="24">
-        <v>3543.75</v>
-      </c>
-      <c r="I6" s="12"/>
-      <c r="L6" s="32"/>
+      <c r="H6" s="32">
+        <v>27168.75</v>
+      </c>
+      <c r="K6" s="32"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
@@ -4396,11 +4391,10 @@
       <c r="G7" s="22">
         <v>27000</v>
       </c>
-      <c r="H7" s="24">
-        <v>4050</v>
-      </c>
-      <c r="I7" s="12"/>
-      <c r="L7" s="32"/>
+      <c r="H7" s="32">
+        <v>31050</v>
+      </c>
+      <c r="K7" s="32"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
@@ -4424,11 +4418,10 @@
       <c r="G8" s="22">
         <v>30375</v>
       </c>
-      <c r="H8" s="24">
-        <v>4556.25</v>
-      </c>
-      <c r="I8" s="12"/>
-      <c r="L8" s="32"/>
+      <c r="H8" s="32">
+        <v>34931.25</v>
+      </c>
+      <c r="K8" s="32"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
@@ -4452,11 +4445,10 @@
       <c r="G9" s="22">
         <v>33750</v>
       </c>
-      <c r="H9" s="24">
-        <v>5062.5</v>
-      </c>
-      <c r="I9" s="12"/>
-      <c r="L9" s="32"/>
+      <c r="H9" s="32">
+        <v>38812.5</v>
+      </c>
+      <c r="K9" s="32"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L10" s="32"/>
@@ -4472,8 +4464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD2F7729-FAD2-491C-95C0-EDC985E8B8AE}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>